<commit_message>
replace excel files with updated files
</commit_message>
<xml_diff>
--- a/assets/Arabic-Overactive-Bladder-My-Bladder-Diary.xlsx
+++ b/assets/Arabic-Overactive-Bladder-My-Bladder-Diary.xlsx
@@ -8,104 +8,123 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amrhussein/Triangles Clients/SAJA/Mohamed Ghonim/OAB Web app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA006D4B-895F-124D-B4FC-9C7C3821AA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EBE19C-743A-C64B-9312-0B678807AF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="560" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_C0F364CE_5427_4F5F_8712_7AA3601F4F62_.wvu.FilterData" localSheetId="0">Sheet1!$B$3:$I$7</definedName>
+    <definedName name="Z_C0F364CE_5427_4F5F_8712_7AA3601F4F62_.wvu.FilterData" localSheetId="0">Sheet1!$B$3:$I$8</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
-    <t>Example</t>
+    <t>(OAB) تقييم أعراض فرط نشاط المثانة</t>
   </si>
   <si>
-    <t>جدول يوميات فرط نشاط المثانة</t>
+    <t>يرجى استخدام هذه المفكرة لتسجيل عادات التبول</t>
   </si>
   <si>
-    <t>قد يساعدك الاحتفاظ بمفكرة يومية فرط نشاط المثانة 
- ومقدم الرعاية الصحية الخاص بك على فهم أعراض الجهاز البولي.</t>
+    <t>التاريخ</t>
+  </si>
+  <si>
+    <t>يوم /شهر/سنة</t>
+  </si>
+  <si>
+    <t>السوائل</t>
+  </si>
+  <si>
+    <t>التبول</t>
+  </si>
+  <si>
+    <t>حوادث</t>
+  </si>
+  <si>
+    <t>ما نوع السائل؟</t>
+  </si>
+  <si>
+    <t>كم تبلغ الكمية؟</t>
+  </si>
+  <si>
+    <t>كم عدد المرات؟</t>
+  </si>
+  <si>
+    <t>هل شعرت
+برغبة شديدة
+في التبول؟</t>
+  </si>
+  <si>
+    <t>ما النشاط الذي تسبب التبول في إيقافه؟</t>
+  </si>
+  <si>
+    <t>هل حدث وتبولت لا إراديًا؟</t>
+  </si>
+  <si>
+    <t>ما هي كمية التسرب؟</t>
+  </si>
+  <si>
+    <t>ما الذي كنت تفعله في ذلك الوقت؟</t>
+  </si>
+  <si>
+    <t>٦-٩ صباحاً</t>
+  </si>
+  <si>
+    <t>٩ صباحاً - ١٢ مساءً</t>
+  </si>
+  <si>
+    <t>١٢ - ٣ مساءً</t>
+  </si>
+  <si>
+    <t>٣ - ٦ مساءً</t>
+  </si>
+  <si>
+    <t>٦ - ٩ مساءً</t>
+  </si>
+  <si>
+    <t>٩ مساءً - ١٢ صباحاً</t>
+  </si>
+  <si>
+    <t>١٢ صباحاً - ٣ صباحاً</t>
+  </si>
+  <si>
+    <t>٣ صباحاً - ٦ صباحاً</t>
+  </si>
+  <si>
+    <t>نعم • لا</t>
+  </si>
+  <si>
+    <t>صغير • متوسط • كبير</t>
+  </si>
+  <si>
+    <t>اليوم الأول</t>
+  </si>
+  <si>
+    <t>اليوم الثاني</t>
+  </si>
+  <si>
+    <t>اليوم الثالث</t>
+  </si>
+  <si>
+    <t>قم بتحميل تطبيق google sheet أو excel لإستخدام هذه المفكرة لتسجيل عادات التبول</t>
   </si>
   <si>
     <t>الوقت</t>
-  </si>
-  <si>
-    <t>المشروبات</t>
-  </si>
-  <si>
-    <t>التسريبات العرضية</t>
-  </si>
-  <si>
-    <t>هل شعرت برغبة قوية في الذهاب؟</t>
-  </si>
-  <si>
-    <t>ماذا كنت تفعل في ذلك الوقت؟</t>
-  </si>
-  <si>
-    <t>النوع ؟</t>
-  </si>
-  <si>
-    <t>الكمية ؟</t>
-  </si>
-  <si>
-    <t>عدد المرات ؟</t>
-  </si>
-  <si>
-    <t>كمية البول ؟</t>
-  </si>
-  <si>
-    <t>نعم / لا</t>
-  </si>
-  <si>
-    <t>العطس وممارسة الرياضة
-وما إلى ذلك.</t>
-  </si>
-  <si>
-    <t>ضحك</t>
-  </si>
-  <si>
-    <t>لا</t>
-  </si>
-  <si>
-    <t>نعم - 
-كمية كبيرة</t>
-  </si>
-  <si>
-    <t>ذهابك إلى الحمام</t>
-  </si>
-  <si>
-    <t>٥٠٠ مل</t>
-  </si>
-  <si>
-    <t>مياه غازية</t>
-  </si>
-  <si>
-    <t>٢-٣ مساءً</t>
-  </si>
-  <si>
-    <t>٣٥٠ مل</t>
-  </si>
-  <si>
-    <t>قم بتحميل تطبيق جوجل شيت او اكسيل</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h&quot;:&quot;mm&quot; &quot;AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[$-2000401]0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -217,14 +236,51 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color rgb="FF000000"/>
+      <name val="Merriweather"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Merriweather"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Merriweather"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Merriweather"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Merriweather"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,8 +353,26 @@
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF942093"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -323,64 +397,29 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -388,24 +427,33 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -429,7 +477,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -443,62 +491,47 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="164" fontId="22" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="164" fontId="22" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="164" fontId="22" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -523,6 +556,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF942093"/>
+      <color rgb="FFFF40FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -831,30 +870,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1002"/>
+  <dimension ref="A1:AA998"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:I38"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" customWidth="1"/>
-    <col min="11" max="1024" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="1024" width="13.42578125" customWidth="1"/>
     <col min="1025" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -862,9 +903,9 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -882,20 +923,20 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="15" t="s">
-        <v>2</v>
+      <c r="B2" s="14" t="s">
+        <v>1</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -913,30 +954,26 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
-    <row r="3" spans="1:27" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
-      <c r="B3" s="22" t="s">
-        <v>3</v>
+      <c r="B3" s="17" t="s">
+        <v>2</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="9" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -954,32 +991,20 @@
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
     </row>
-    <row r="4" spans="1:27" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="18" t="s">
-        <v>8</v>
+    <row r="4" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="15" t="s">
+        <v>3</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -997,36 +1022,38 @@
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
     </row>
-    <row r="5" spans="1:27" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>0</v>
+    <row r="5" spans="1:27" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="18" t="s">
+        <v>29</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>20</v>
+      <c r="C5" s="18" t="s">
+        <v>7</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>19</v>
+      <c r="D5" s="18" t="s">
+        <v>8</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>18</v>
+      <c r="E5" s="18" t="s">
+        <v>9</v>
       </c>
-      <c r="E5" s="21">
-        <v>4</v>
+      <c r="F5" s="18" t="s">
+        <v>8</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>21</v>
+      <c r="G5" s="18" t="s">
+        <v>10</v>
       </c>
-      <c r="G5" s="20" t="s">
-        <v>16</v>
+      <c r="H5" s="18" t="s">
+        <v>11</v>
       </c>
-      <c r="H5" s="20" t="s">
-        <v>15</v>
+      <c r="I5" s="18" t="s">
+        <v>12</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="J5" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1044,18 +1071,20 @@
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
     </row>
-    <row r="6" spans="1:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+    <row r="6" spans="1:27" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1073,18 +1102,26 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
     </row>
-    <row r="7" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="8"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1102,18 +1139,20 @@
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
     </row>
-    <row r="8" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1131,18 +1170,20 @@
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
     </row>
-    <row r="9" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1160,18 +1201,20 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="B10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1189,18 +1232,20 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
     </row>
-    <row r="11" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1218,18 +1263,20 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1247,18 +1294,20 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
     </row>
-    <row r="13" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="B13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1276,18 +1325,20 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="B14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1305,18 +1356,20 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="B15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1334,18 +1387,20 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="25" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="B16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1363,18 +1418,20 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
     </row>
-    <row r="17" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1392,18 +1449,20 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
-    <row r="18" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="B18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1421,18 +1480,20 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="B19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1450,18 +1511,20 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
     </row>
-    <row r="20" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="B20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -1479,18 +1542,20 @@
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
     </row>
-    <row r="21" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="B21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1508,18 +1573,20 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="B22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1537,18 +1604,20 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
+      <c r="B23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1566,18 +1635,20 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
     </row>
-    <row r="24" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="B24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -1595,18 +1666,20 @@
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
     </row>
-    <row r="25" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="B25" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="11"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1624,18 +1697,20 @@
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
     </row>
-    <row r="26" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="B26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1653,18 +1728,20 @@
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
     </row>
-    <row r="27" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="B27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -1682,18 +1759,20 @@
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
     </row>
-    <row r="28" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="B28" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -1711,18 +1790,20 @@
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
     </row>
-    <row r="29" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="B29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -1740,18 +1821,20 @@
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
     </row>
-    <row r="30" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="B30" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -1769,18 +1852,20 @@
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
     </row>
-    <row r="31" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="B31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -1798,18 +1883,20 @@
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
     </row>
-    <row r="32" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="B32" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -1827,18 +1914,20 @@
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
     </row>
-    <row r="33" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+      <c r="B33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -1856,18 +1945,20 @@
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
     </row>
-    <row r="34" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="B34" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -1887,14 +1978,14 @@
     </row>
     <row r="35" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -1916,14 +2007,14 @@
     </row>
     <row r="36" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -1945,14 +2036,14 @@
     </row>
     <row r="37" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -1972,18 +2063,16 @@
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
     </row>
-    <row r="38" spans="1:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -29843,131 +29932,19 @@
       <c r="Z998" s="2"/>
       <c r="AA998" s="2"/>
     </row>
-    <row r="999" spans="1:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="A999" s="2"/>
-      <c r="B999" s="2"/>
-      <c r="C999" s="2"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="2"/>
-      <c r="F999" s="2"/>
-      <c r="G999" s="2"/>
-      <c r="H999" s="2"/>
-      <c r="I999" s="2"/>
-      <c r="J999" s="2"/>
-      <c r="K999" s="2"/>
-      <c r="L999" s="2"/>
-      <c r="M999" s="2"/>
-      <c r="N999" s="2"/>
-      <c r="O999" s="2"/>
-      <c r="P999" s="2"/>
-      <c r="Q999" s="2"/>
-      <c r="R999" s="2"/>
-      <c r="S999" s="2"/>
-      <c r="T999" s="2"/>
-      <c r="U999" s="2"/>
-      <c r="V999" s="2"/>
-      <c r="W999" s="2"/>
-      <c r="X999" s="2"/>
-      <c r="Y999" s="2"/>
-      <c r="Z999" s="2"/>
-      <c r="AA999" s="2"/>
-    </row>
-    <row r="1000" spans="1:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1000" s="2"/>
-      <c r="B1000" s="2"/>
-      <c r="C1000" s="2"/>
-      <c r="D1000" s="2"/>
-      <c r="E1000" s="2"/>
-      <c r="F1000" s="2"/>
-      <c r="G1000" s="2"/>
-      <c r="H1000" s="2"/>
-      <c r="I1000" s="2"/>
-      <c r="J1000" s="2"/>
-      <c r="K1000" s="2"/>
-      <c r="L1000" s="2"/>
-      <c r="M1000" s="2"/>
-      <c r="N1000" s="2"/>
-      <c r="O1000" s="2"/>
-      <c r="P1000" s="2"/>
-      <c r="Q1000" s="2"/>
-      <c r="R1000" s="2"/>
-      <c r="S1000" s="2"/>
-      <c r="T1000" s="2"/>
-      <c r="U1000" s="2"/>
-      <c r="V1000" s="2"/>
-      <c r="W1000" s="2"/>
-      <c r="X1000" s="2"/>
-      <c r="Y1000" s="2"/>
-      <c r="Z1000" s="2"/>
-      <c r="AA1000" s="2"/>
-    </row>
-    <row r="1001" spans="1:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1001" s="2"/>
-      <c r="B1001" s="2"/>
-      <c r="C1001" s="2"/>
-      <c r="D1001" s="2"/>
-      <c r="E1001" s="2"/>
-      <c r="F1001" s="2"/>
-      <c r="G1001" s="2"/>
-      <c r="H1001" s="2"/>
-      <c r="I1001" s="2"/>
-      <c r="J1001" s="2"/>
-      <c r="K1001" s="2"/>
-      <c r="L1001" s="2"/>
-      <c r="M1001" s="2"/>
-      <c r="N1001" s="2"/>
-      <c r="O1001" s="2"/>
-      <c r="P1001" s="2"/>
-      <c r="Q1001" s="2"/>
-      <c r="R1001" s="2"/>
-      <c r="S1001" s="2"/>
-      <c r="T1001" s="2"/>
-      <c r="U1001" s="2"/>
-      <c r="V1001" s="2"/>
-      <c r="W1001" s="2"/>
-      <c r="X1001" s="2"/>
-      <c r="Y1001" s="2"/>
-      <c r="Z1001" s="2"/>
-      <c r="AA1001" s="2"/>
-    </row>
-    <row r="1002" spans="1:27" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1002" s="2"/>
-      <c r="B1002" s="2"/>
-      <c r="C1002" s="2"/>
-      <c r="D1002" s="2"/>
-      <c r="E1002" s="2"/>
-      <c r="F1002" s="2"/>
-      <c r="G1002" s="2"/>
-      <c r="H1002" s="2"/>
-      <c r="I1002" s="2"/>
-      <c r="J1002" s="2"/>
-      <c r="K1002" s="2"/>
-      <c r="L1002" s="2"/>
-      <c r="M1002" s="2"/>
-      <c r="N1002" s="2"/>
-      <c r="O1002" s="2"/>
-      <c r="P1002" s="2"/>
-      <c r="Q1002" s="2"/>
-      <c r="R1002" s="2"/>
-      <c r="S1002" s="2"/>
-      <c r="T1002" s="2"/>
-      <c r="U1002" s="2"/>
-      <c r="V1002" s="2"/>
-      <c r="W1002" s="2"/>
-      <c r="X1002" s="2"/>
-      <c r="Y1002" s="2"/>
-      <c r="Z1002" s="2"/>
-      <c r="AA1002" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="B3:B4"/>
+  <mergeCells count="9">
+    <mergeCell ref="B25:K25"/>
+    <mergeCell ref="B34:K34"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="E3:H4"/>
+    <mergeCell ref="I3:K4"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B16:K16"/>
   </mergeCells>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.74805555555555614" right="0.74805555555555614" top="1.3776388888888891" bottom="1.3776388888888891" header="0.98388888888888903" footer="0.98388888888888903"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>